<commit_message>
add new fields: alternate_ids, status, etc.
</commit_message>
<xml_diff>
--- a/schema/rpoc/excel/rpoc.xlsx
+++ b/schema/rpoc/excel/rpoc.xlsx
@@ -593,203 +593,198 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>primary_email</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nick</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>avatar</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_employment_history</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>aliases</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>primary_email</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>purpose_statement</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>start_date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>current_address</t>
+          <t>end_date</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>position</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nick</t>
+          <t>aliases</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>avatar</t>
+          <t>id</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>has_employment_history</t>
+          <t>name</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>aliases</t>
+          <t>description</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
+          <t>image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>role_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>role_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"nonbinary man,nonbinary woman,transgender woman,transgender man,cisgender man,cisgender woman"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>mission_statement</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>start_date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>end_date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>parent</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>aliases</t>
+          <t>status</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>role_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>role_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>start_date</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>end_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
         <is>
           <t>aliases</t>
         </is>
@@ -811,7 +806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -847,6 +842,11 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>

</xml_diff>